<commit_message>
added new olc contracts
</commit_message>
<xml_diff>
--- a/public/ethiopian-contracts/data/excels/ADA%20Commercial%20Inc._Liberia.xlsx
+++ b/public/ethiopian-contracts/data/excels/ADA%20Commercial%20Inc._Liberia.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="540" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16806" uniqueCount="16775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16806" uniqueCount="16776">
   <si>
     <t>17 (middle)</t>
     <phoneticPr fontId="11" type="noConversion"/>
@@ -50292,9 +50292,6 @@
   </si>
   <si>
     <t>Rice products in quantities deemed appropriate by ADA Commercial</t>
-  </si>
-  <si>
-    <t>Twenty years, commencing on the contract's effective date and ending 240 calendar months after</t>
   </si>
   <si>
     <t>Upon the request of the Government, ADA Commercial will consult on community plans and programs and will cooperate to realize such programs. In addition, ADA Commercial will provide advisory support and, subject to availability, farm supplies to qualified Liberian rice farmers, to include seed rice, seeders, and fertilizers, at charges no greater than ADA Commercial's own cost for such items, including any taxes and duties. Each year during the term of the contract, ADA Commercial shall submit a rolling 5-year development plan, which will include details on the outgrowers program.</t>
@@ -50394,11 +50391,20 @@
   <si>
     <t>Concession Agreement</t>
   </si>
+  <si>
+    <t>20 years</t>
+  </si>
+  <si>
+    <t>Rice, Rice products</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -51119,9 +51125,6 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -51166,6 +51169,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -51175,7 +51181,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -51532,8 +51538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -101026,7 +101032,7 @@
       <c r="B17" s="11" t="s">
         <v>16691</v>
       </c>
-      <c r="C17" s="170">
+      <c r="C17" s="169">
         <v>39758</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -101304,7 +101310,7 @@
       <c r="B29" s="89" t="s">
         <v>16603</v>
       </c>
-      <c r="C29" s="166">
+      <c r="C29" s="186">
         <v>39572</v>
       </c>
       <c r="D29" s="164" t="s">
@@ -101357,7 +101363,7 @@
         <v>16645</v>
       </c>
       <c r="C31" s="164" t="s">
-        <v>16743</v>
+        <v>16774</v>
       </c>
       <c r="D31" s="164" t="s">
         <v>16615</v>
@@ -101372,7 +101378,7 @@
       </c>
       <c r="H31" s="92" t="str">
         <f t="shared" si="0"/>
-        <v>Twenty years, commencing on the contract's effective date and ending 240 calendar months after--Art. 2</v>
+        <v>20 years--Art. 2</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="84" customFormat="1" ht="135">
@@ -101409,7 +101415,7 @@
         <v>16382</v>
       </c>
       <c r="C33" s="164" t="s">
-        <v>16695</v>
+        <v>16775</v>
       </c>
       <c r="D33" s="164" t="s">
         <v>16696</v>
@@ -101424,7 +101430,7 @@
       </c>
       <c r="H33" s="92" t="str">
         <f t="shared" si="0"/>
-        <v>Rice and rice products--Art. 3.1</v>
+        <v>Rice, Rice products--Art. 3.1</v>
       </c>
     </row>
     <row r="34" spans="1:25" s="93" customFormat="1" ht="60">
@@ -101497,7 +101503,7 @@
         <v>16531</v>
       </c>
       <c r="C37" s="164" t="s">
-        <v>16744</v>
+        <v>16743</v>
       </c>
       <c r="D37" s="164" t="s">
         <v>16702</v>
@@ -101654,7 +101660,7 @@
         <v>16537</v>
       </c>
       <c r="C42" s="165" t="s">
-        <v>16745</v>
+        <v>16744</v>
       </c>
       <c r="D42" s="165" t="s">
         <v>16635</v>
@@ -101697,7 +101703,7 @@
         <v>16539</v>
       </c>
       <c r="C43" s="164" t="s">
-        <v>16746</v>
+        <v>16745</v>
       </c>
       <c r="D43" s="164" t="s">
         <v>16640</v>
@@ -101740,7 +101746,7 @@
         <v>16541</v>
       </c>
       <c r="C44" s="164" t="s">
-        <v>16747</v>
+        <v>16746</v>
       </c>
       <c r="D44" s="164" t="s">
         <v>16638</v>
@@ -101783,10 +101789,10 @@
         <v>16365</v>
       </c>
       <c r="C45" s="94" t="s">
+        <v>16747</v>
+      </c>
+      <c r="D45" s="94" t="s">
         <v>16748</v>
-      </c>
-      <c r="D45" s="94" t="s">
-        <v>16749</v>
       </c>
       <c r="E45" s="94" t="s">
         <v>16701</v>
@@ -101900,7 +101906,7 @@
         <v>16366</v>
       </c>
       <c r="C48" s="165" t="s">
-        <v>16750</v>
+        <v>16749</v>
       </c>
       <c r="D48" s="165" t="s">
         <v>16720</v>
@@ -101942,8 +101948,8 @@
       <c r="B49" s="105" t="s">
         <v>16367</v>
       </c>
-      <c r="C49" s="179" t="s">
-        <v>16759</v>
+      <c r="C49" s="178" t="s">
+        <v>16758</v>
       </c>
       <c r="D49" s="105" t="s">
         <v>16721</v>
@@ -101986,10 +101992,10 @@
         <v>16319</v>
       </c>
       <c r="C50" s="165" t="s">
-        <v>16751</v>
+        <v>16750</v>
       </c>
       <c r="D50" s="165" t="s">
-        <v>16760</v>
+        <v>16759</v>
       </c>
       <c r="E50" s="165" t="s">
         <v>16704</v>
@@ -102072,7 +102078,7 @@
         <v>16321</v>
       </c>
       <c r="C52" s="105" t="s">
-        <v>16752</v>
+        <v>16751</v>
       </c>
       <c r="D52" s="105" t="s">
         <v>16677</v>
@@ -102244,13 +102250,13 @@
       <c r="B58" s="116" t="s">
         <v>16551</v>
       </c>
-      <c r="C58" s="168" t="s">
+      <c r="C58" s="167" t="s">
         <v>16707</v>
       </c>
-      <c r="D58" s="168" t="s">
+      <c r="D58" s="167" t="s">
         <v>16706</v>
       </c>
-      <c r="E58" s="168" t="s">
+      <c r="E58" s="167" t="s">
         <v>16653</v>
       </c>
       <c r="F58" s="119"/>
@@ -102290,13 +102296,13 @@
       <c r="B60" s="116" t="s">
         <v>16618</v>
       </c>
-      <c r="C60" s="178" t="s">
-        <v>16753</v>
-      </c>
-      <c r="D60" s="168" t="s">
+      <c r="C60" s="177" t="s">
+        <v>16752</v>
+      </c>
+      <c r="D60" s="167" t="s">
         <v>16735</v>
       </c>
-      <c r="E60" s="168" t="s">
+      <c r="E60" s="167" t="s">
         <v>16736</v>
       </c>
       <c r="F60" s="119"/>
@@ -102436,8 +102442,8 @@
       <c r="B67" s="30" t="s">
         <v>16491</v>
       </c>
-      <c r="C67" s="180" t="s">
-        <v>16769</v>
+      <c r="C67" s="179" t="s">
+        <v>16768</v>
       </c>
       <c r="D67" s="30" t="s">
         <v>16708</v>
@@ -102609,7 +102615,7 @@
         <v>16507</v>
       </c>
       <c r="C75" s="41" t="s">
-        <v>16770</v>
+        <v>16769</v>
       </c>
       <c r="D75" s="30" t="s">
         <v>16710</v>
@@ -102693,7 +102699,7 @@
         <v>16517</v>
       </c>
       <c r="C79" s="30" t="s">
-        <v>16754</v>
+        <v>16753</v>
       </c>
       <c r="D79" s="30" t="s">
         <v>16712</v>
@@ -102758,13 +102764,13 @@
       <c r="B82" s="122" t="s">
         <v>16521</v>
       </c>
-      <c r="C82" s="173" t="s">
+      <c r="C82" s="172" t="s">
         <v>16717</v>
       </c>
-      <c r="D82" s="172" t="s">
+      <c r="D82" s="171" t="s">
         <v>16652</v>
       </c>
-      <c r="E82" s="171" t="s">
+      <c r="E82" s="170" t="s">
         <v>16651</v>
       </c>
       <c r="F82" s="123"/>
@@ -102785,7 +102791,7 @@
         <v>16524</v>
       </c>
       <c r="C83" s="30" t="s">
-        <v>16755</v>
+        <v>16754</v>
       </c>
       <c r="D83" s="30" t="s">
         <v>16737</v>
@@ -102890,13 +102896,13 @@
       <c r="B88" s="116" t="s">
         <v>16413</v>
       </c>
-      <c r="C88" s="168" t="s">
-        <v>16756</v>
-      </c>
-      <c r="D88" s="168" t="s">
+      <c r="C88" s="167" t="s">
+        <v>16755</v>
+      </c>
+      <c r="D88" s="167" t="s">
         <v>16648</v>
       </c>
-      <c r="E88" s="168" t="s">
+      <c r="E88" s="167" t="s">
         <v>16679</v>
       </c>
       <c r="F88" s="119"/>
@@ -102916,13 +102922,13 @@
       <c r="B89" s="116" t="s">
         <v>16415</v>
       </c>
-      <c r="C89" s="168" t="s">
-        <v>16768</v>
-      </c>
-      <c r="D89" s="168" t="s">
+      <c r="C89" s="167" t="s">
+        <v>16767</v>
+      </c>
+      <c r="D89" s="167" t="s">
         <v>16680</v>
       </c>
-      <c r="E89" s="168" t="s">
+      <c r="E89" s="167" t="s">
         <v>16641</v>
       </c>
       <c r="F89" s="119"/>
@@ -102942,13 +102948,13 @@
       <c r="B90" s="113" t="s">
         <v>16738</v>
       </c>
-      <c r="C90" s="178" t="s">
+      <c r="C90" s="177" t="s">
         <v>16740</v>
       </c>
-      <c r="D90" s="178" t="s">
+      <c r="D90" s="177" t="s">
         <v>16739</v>
       </c>
-      <c r="E90" s="182" t="s">
+      <c r="E90" s="181" t="s">
         <v>16709</v>
       </c>
       <c r="F90" s="119"/>
@@ -103065,12 +103071,12 @@
         <v>16370</v>
       </c>
       <c r="C96" s="165" t="s">
-        <v>16757</v>
+        <v>16756</v>
       </c>
       <c r="D96" s="165" t="s">
         <v>16649</v>
       </c>
-      <c r="E96" s="167" t="s">
+      <c r="E96" s="166" t="s">
         <v>16650</v>
       </c>
       <c r="F96" s="12"/>
@@ -103091,7 +103097,7 @@
         <v>16314</v>
       </c>
       <c r="C97" s="113" t="s">
-        <v>16758</v>
+        <v>16757</v>
       </c>
       <c r="D97" s="113" t="s">
         <v>16718</v>
@@ -103294,7 +103300,7 @@
       </c>
       <c r="C107" s="165"/>
       <c r="D107" s="165"/>
-      <c r="E107" s="167"/>
+      <c r="E107" s="166"/>
       <c r="F107" s="12"/>
       <c r="G107" s="13" t="str">
         <f>IF(OR(Categories!$B107&lt;&gt;"",Categories!$A107&lt;&gt;""),Categories!$A107&amp;"//"&amp;Categories!$B107,"")</f>
@@ -103313,7 +103319,7 @@
         <v>16431</v>
       </c>
       <c r="C108" s="165" t="s">
-        <v>16771</v>
+        <v>16770</v>
       </c>
       <c r="D108" s="165" t="s">
         <v>16684</v>
@@ -103359,8 +103365,8 @@
         <v>16413</v>
       </c>
       <c r="C110" s="165"/>
-      <c r="D110" s="174"/>
-      <c r="E110" s="175"/>
+      <c r="D110" s="173"/>
+      <c r="E110" s="174"/>
       <c r="F110" s="33"/>
       <c r="G110" s="34" t="str">
         <f>IF(OR(Categories!$B110&lt;&gt;"",Categories!$A110&lt;&gt;""),Categories!$A110&amp;"//"&amp;Categories!$B110,"")</f>
@@ -103379,7 +103385,7 @@
         <v>16372</v>
       </c>
       <c r="C111" s="113" t="s">
-        <v>16772</v>
+        <v>16771</v>
       </c>
       <c r="D111" s="113" t="s">
         <v>16725</v>
@@ -103405,7 +103411,7 @@
         <v>16373</v>
       </c>
       <c r="C112" s="113" t="s">
-        <v>16773</v>
+        <v>16772</v>
       </c>
       <c r="D112" s="113" t="s">
         <v>16723</v>
@@ -103451,7 +103457,7 @@
         <v>16314</v>
       </c>
       <c r="C114" s="113" t="s">
-        <v>16758</v>
+        <v>16757</v>
       </c>
       <c r="D114" s="142" t="s">
         <v>16718</v>
@@ -103538,10 +103544,10 @@
       <c r="D118" s="164" t="s">
         <v>16681</v>
       </c>
-      <c r="E118" s="169" t="s">
+      <c r="E118" s="168" t="s">
         <v>16664</v>
       </c>
-      <c r="F118" s="169"/>
+      <c r="F118" s="168"/>
       <c r="G118" s="91" t="str">
         <f>IF(OR(Categories!$B118&lt;&gt;"",Categories!$A118&lt;&gt;""),Categories!$A118&amp;"//"&amp;Categories!$B118,"")</f>
         <v>Loi applicable en cas des différends//Governing law in case of dispute</v>
@@ -103558,7 +103564,7 @@
       <c r="B119" s="116" t="s">
         <v>16439</v>
       </c>
-      <c r="C119" s="177" t="s">
+      <c r="C119" s="176" t="s">
         <v>16729</v>
       </c>
       <c r="D119" s="164" t="s">
@@ -103584,7 +103590,7 @@
       <c r="B120" s="132" t="s">
         <v>16441</v>
       </c>
-      <c r="C120" s="179" t="s">
+      <c r="C120" s="178" t="s">
         <v>16730</v>
       </c>
       <c r="D120" s="94" t="s">
@@ -103611,7 +103617,7 @@
         <v>16443</v>
       </c>
       <c r="C121" s="36" t="s">
-        <v>16762</v>
+        <v>16761</v>
       </c>
       <c r="D121" s="11" t="s">
         <v>16733</v>
@@ -103637,7 +103643,7 @@
         <v>16445</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>16761</v>
+        <v>16760</v>
       </c>
       <c r="D122" s="165" t="s">
         <v>16683</v>
@@ -103663,12 +103669,12 @@
         <v>16447</v>
       </c>
       <c r="C123" s="36" t="s">
-        <v>16763</v>
+        <v>16762</v>
       </c>
       <c r="D123" s="165" t="s">
         <v>16662</v>
       </c>
-      <c r="E123" s="167" t="s">
+      <c r="E123" s="166" t="s">
         <v>16663</v>
       </c>
       <c r="F123" s="12"/>
@@ -103688,8 +103694,8 @@
       <c r="B124" s="105" t="s">
         <v>16556</v>
       </c>
-      <c r="C124" s="176" t="s">
-        <v>16764</v>
+      <c r="C124" s="175" t="s">
+        <v>16763</v>
       </c>
       <c r="D124" s="164" t="s">
         <v>2</v>
@@ -103714,7 +103720,7 @@
       <c r="B125" s="105" t="s">
         <v>16558</v>
       </c>
-      <c r="C125" s="181" t="s">
+      <c r="C125" s="180" t="s">
         <v>16623</v>
       </c>
       <c r="D125" s="89"/>
@@ -103737,7 +103743,7 @@
         <v>16324</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>16765</v>
+        <v>16764</v>
       </c>
       <c r="D126" s="11" t="s">
         <v>1</v>
@@ -103781,7 +103787,7 @@
         <v>16377</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>16766</v>
+        <v>16765</v>
       </c>
       <c r="D128" s="11" t="s">
         <v>16665</v>
@@ -103807,7 +103813,7 @@
         <v>16376</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>16767</v>
+        <v>16766</v>
       </c>
       <c r="D129" s="11" t="s">
         <v>16658</v>
@@ -104051,14 +104057,14 @@
         <v>16482</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16774</v>
+        <v>16773</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="63" t="s">
         <v>16361</v>
       </c>
-      <c r="B5" s="186">
+      <c r="B5" s="182">
         <v>39572</v>
       </c>
     </row>

</xml_diff>